<commit_message>
commit by Swati on 4/25/18
</commit_message>
<xml_diff>
--- a/FindLawTest/src/test/resources/testdata/TestData.xlsx
+++ b/FindLawTest/src/test/resources/testdata/TestData.xlsx
@@ -33,9 +33,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>rishu.kumari@thomsonreuters.com.lrp1qa1</t>
-  </si>
-  <si>
     <t>Record</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
     <t>Administrative Law</t>
   </si>
   <si>
-    <t>Pass@1709</t>
-  </si>
-  <si>
     <t>Q-00045061</t>
   </si>
   <si>
@@ -325,13 +319,19 @@
   </si>
   <si>
     <t>Sales_Rep</t>
+  </si>
+  <si>
+    <t>swati.chetty@thomsonreuters.com.lrp5qa</t>
+  </si>
+  <si>
+    <t>March12345</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,6 +352,14 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -370,10 +378,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -384,8 +393,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -691,7 +702,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,65 +727,68 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
       </c>
       <c r="E2">
         <v>9100002</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
         <v>72</v>
       </c>
-      <c r="H2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" t="s">
-        <v>74</v>
-      </c>
       <c r="J2" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -799,13 +813,13 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -849,19 +863,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -869,22 +883,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -911,18 +925,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -948,24 +962,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -996,28 +1010,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
       <c r="D1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1118,7 +1132,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1160,144 +1174,144 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
       <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" t="s">
         <v>55</v>
       </c>
-      <c r="L1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O1" t="s">
-        <v>55</v>
-      </c>
-      <c r="P1" t="s">
-        <v>56</v>
-      </c>
       <c r="Q1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" t="s">
         <v>58</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>59</v>
       </c>
-      <c r="S1" t="s">
-        <v>60</v>
-      </c>
       <c r="T1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U1" t="s">
+        <v>88</v>
+      </c>
+      <c r="V1" t="s">
         <v>90</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>92</v>
-      </c>
-      <c r="W1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>9032479759</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
         <v>66</v>
       </c>
-      <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" t="s">
+        <v>61</v>
+      </c>
+      <c r="P2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" t="s">
         <v>47</v>
       </c>
-      <c r="K2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" t="s">
-        <v>54</v>
-      </c>
-      <c r="O2" t="s">
-        <v>62</v>
-      </c>
-      <c r="P2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>48</v>
-      </c>
       <c r="R2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="T2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="U2" t="s">
+        <v>89</v>
+      </c>
+      <c r="V2" t="s">
         <v>91</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>93</v>
-      </c>
-      <c r="W2" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1322,42 +1336,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
         <v>81</v>
-      </c>
-      <c r="E1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" t="s">
         <v>84</v>
-      </c>
-      <c r="E2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>